<commit_message>
Abstract classes + interfaces
</commit_message>
<xml_diff>
--- a/workload repartition.xlsx
+++ b/workload repartition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alpha/switchdrive/ACT-TP/act-github/act-tp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEAE778-5346-7D47-98C1-005F3A9537EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F38F64-8B9E-974F-B810-253D6F62810A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,13 +639,12 @@
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="Q7" sqref="Q7"/>
-      <selection pane="topRight" activeCell="G19" sqref="G19"/>
+      <selection pane="topRight" activeCell="B1" sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="1" max="2" width="4.83203125" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Question 5.2 - comments translated
</commit_message>
<xml_diff>
--- a/workload repartition.xlsx
+++ b/workload repartition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alpha/switchdrive/ACT-TP/act-github/act-tp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F38F64-8B9E-974F-B810-253D6F62810A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29649E9E-8699-AD43-BF81-5603F7659C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="500" windowWidth="32120" windowHeight="20960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -639,12 +639,12 @@
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="Q7" sqref="Q7"/>
-      <selection pane="topRight" activeCell="B1" sqref="A1:B1048576"/>
+      <selection pane="topRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="4.83203125" customWidth="1"/>
+    <col min="1" max="2" width="4.83203125" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.33203125" customWidth="1"/>
     <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>

</xml_diff>